<commit_message>
New approach to asking questions
</commit_message>
<xml_diff>
--- a/media/files/skills.xlsx
+++ b/media/files/skills.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/afb61024139a389c/Hobbies/Django/Skills/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C26FE7B-3FBD-43DF-8702-2C1F5D62FEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="237" documentId="8_{8C26FE7B-3FBD-43DF-8702-2C1F5D62FEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{359A43B1-1C83-4970-9968-26D8B46E9CB0}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{2538A450-F464-4C67-8C17-3CEAE73EC98F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Full List" sheetId="1" r:id="rId1"/>
-    <sheet name="Mapped to areas" sheetId="2" r:id="rId2"/>
+    <sheet name="Questions" sheetId="3" r:id="rId1"/>
+    <sheet name="Original questions" sheetId="1" r:id="rId2"/>
+    <sheet name="Questions by area" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,6 +36,71 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Darren Robinson</author>
+  </authors>
+  <commentList>
+    <comment ref="D21" authorId="0" shapeId="0" xr:uid="{46514BC5-25F1-4A41-AD0B-DDC755D61617}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Darren Robinson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Although requirements are developed by 'topic' they would ideally be communicated as a whole to each individual:
+ - What the objective is
+ - What they should do (everything they should do)
+ - How do they do each thing
+ - How do they know each item is complete</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D24" authorId="0" shapeId="0" xr:uid="{54399E8A-46CA-4959-832C-943AB80C63ED}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Darren Robinson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Includes:
+ - Determining whether risks are being managed
+ - Determining whether requirements are being complied with
+ - Identifying the need for and implementing targeted deep dives</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Darren Robinson</author>
@@ -173,7 +239,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1176" uniqueCount="309">
   <si>
     <t>Expert</t>
   </si>
@@ -711,9 +777,6 @@
     <t>Design and document objectives of training</t>
   </si>
   <si>
-    <t>Define objectives</t>
-  </si>
-  <si>
     <t>Identify risks</t>
   </si>
   <si>
@@ -961,6 +1024,150 @@
   </si>
   <si>
     <t>Highlighted areas in this section relate to support and review not doing.</t>
+  </si>
+  <si>
+    <t>Can guide others</t>
+  </si>
+  <si>
+    <t>Can't do</t>
+  </si>
+  <si>
+    <t>Can do it with guidance</t>
+  </si>
+  <si>
+    <t>Can do it</t>
+  </si>
+  <si>
+    <t>Can review work performed by others</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  and can create XXX</t>
+  </si>
+  <si>
+    <t>Contribute to</t>
+  </si>
+  <si>
+    <t>Define business objectives</t>
+  </si>
+  <si>
+    <t>Develop the team structure</t>
+  </si>
+  <si>
+    <t>Recruit the team</t>
+  </si>
+  <si>
+    <t>Head Of</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>Framework and Governance</t>
+  </si>
+  <si>
+    <t>Requirements (Policies and Procedures)</t>
+  </si>
+  <si>
+    <t>Risk Management Information</t>
+  </si>
+  <si>
+    <t>Line 1 Business Activities - support and review</t>
+  </si>
+  <si>
+    <t>Review business objectives</t>
+  </si>
+  <si>
+    <t>Review processes</t>
+  </si>
+  <si>
+    <t>Review and support the Identification of risks</t>
+  </si>
+  <si>
+    <t>Review and support the assessment of risks (including stress and scenario testing)</t>
+  </si>
+  <si>
+    <t>Review and support the manage of risks</t>
+  </si>
+  <si>
+    <t>Review the testing of controls</t>
+  </si>
+  <si>
+    <t>Review controls</t>
+  </si>
+  <si>
+    <t>Review risk KPIs</t>
+  </si>
+  <si>
+    <t>Review the identification and management of events</t>
+  </si>
+  <si>
+    <t>Review the identification and management of issues</t>
+  </si>
+  <si>
+    <t>Create and run the attestation process</t>
+  </si>
+  <si>
+    <t>Assess attestation responses</t>
+  </si>
+  <si>
+    <t>Review the determination of capital requirements</t>
+  </si>
+  <si>
+    <t>Role_Level</t>
+  </si>
+  <si>
+    <t>Senior Manager</t>
+  </si>
+  <si>
+    <t>Assess effectiveness of the framework and governance</t>
+  </si>
+  <si>
+    <t>Communicate the rationale and requirements of the framework</t>
+  </si>
+  <si>
+    <t>Update the framework and governance</t>
+  </si>
+  <si>
+    <t>Design and write policies and procedures</t>
+  </si>
+  <si>
+    <t>Explain Risk Theory in detail</t>
+  </si>
+  <si>
+    <t>Communicate policies and procedures and how they should be met</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assess Line 1's understanding of the policies andprocedures </t>
+  </si>
+  <si>
+    <t>Assess Line 1's understanding of how to implement policies andprocedures</t>
+  </si>
+  <si>
+    <t>Assess effectiveness of the implementation of policies and procedures</t>
+  </si>
+  <si>
+    <t>Help improve the effectiveness of the implementation of policies and procedures</t>
+  </si>
+  <si>
+    <t>Update and improve the effectiveness of policies and procedures</t>
+  </si>
+  <si>
+    <t>Identify internal and external trends that may present risks and opportunities</t>
+  </si>
+  <si>
+    <t>Design training</t>
+  </si>
+  <si>
+    <t>Deliver training</t>
+  </si>
+  <si>
+    <t>Update training</t>
+  </si>
+  <si>
+    <t>Design and document objectives of the risk management tool</t>
+  </si>
+  <si>
+    <t>Perform user acceptance testing</t>
   </si>
 </sst>
 </file>
@@ -1380,14 +1587,1093 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C32CA44-07D4-4B84-B479-4240FE4261FB}">
+  <dimension ref="A1:H65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E48" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="C56" sqref="C56"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="39.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.1796875" customWidth="1"/>
+    <col min="4" max="4" width="56.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="D2" t="s">
+        <v>269</v>
+      </c>
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D3" t="s">
+        <v>270</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="D4" t="s">
+        <v>208</v>
+      </c>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D5" t="s">
+        <v>209</v>
+      </c>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>166</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="D6" t="s">
+        <v>167</v>
+      </c>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="D7" t="s">
+        <v>182</v>
+      </c>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>166</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="D8" t="s">
+        <v>254</v>
+      </c>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>166</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D9" t="s">
+        <v>168</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D10" t="s">
+        <v>224</v>
+      </c>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D11" t="s">
+        <v>293</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="D12" t="s">
+        <v>292</v>
+      </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="D13" t="s">
+        <v>294</v>
+      </c>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="D14" t="s">
+        <v>185</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="D15" t="s">
+        <v>182</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D16" t="s">
+        <v>223</v>
+      </c>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="D17" t="s">
+        <v>222</v>
+      </c>
+      <c r="F17" s="4"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D18" t="s">
+        <v>186</v>
+      </c>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" t="s">
+        <v>227</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>274</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D20" t="s">
+        <v>295</v>
+      </c>
+      <c r="F20" s="4"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" t="s">
+        <v>274</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D21" t="s">
+        <v>297</v>
+      </c>
+      <c r="E21" s="4"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="4"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" t="s">
+        <v>274</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D22" t="s">
+        <v>298</v>
+      </c>
+      <c r="G22" s="5"/>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>274</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D23" t="s">
+        <v>299</v>
+      </c>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" t="s">
+        <v>274</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D24" t="s">
+        <v>300</v>
+      </c>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" t="s">
+        <v>274</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D25" t="s">
+        <v>301</v>
+      </c>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" t="s">
+        <v>274</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="D26" t="s">
+        <v>170</v>
+      </c>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="5"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" t="s">
+        <v>274</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="D27" t="s">
+        <v>302</v>
+      </c>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="5"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" t="s">
+        <v>197</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D28" t="s">
+        <v>303</v>
+      </c>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" t="s">
+        <v>197</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="D29" t="s">
+        <v>226</v>
+      </c>
+      <c r="G29" s="4"/>
+      <c r="H29" s="5"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" t="s">
+        <v>197</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="D30" t="s">
+        <v>225</v>
+      </c>
+      <c r="G30" s="4"/>
+      <c r="H30" s="5"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D31" t="s">
+        <v>204</v>
+      </c>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D32" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D33" t="s">
+        <v>243</v>
+      </c>
+      <c r="E33" s="5"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D34" t="s">
+        <v>245</v>
+      </c>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D35" t="s">
+        <v>230</v>
+      </c>
+      <c r="E35" s="5"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D36" t="s">
+        <v>244</v>
+      </c>
+      <c r="F36" s="5"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D37" t="s">
+        <v>229</v>
+      </c>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="D38" t="s">
+        <v>256</v>
+      </c>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="5"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="5"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D40" t="s">
+        <v>304</v>
+      </c>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="5"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D41" t="s">
+        <v>305</v>
+      </c>
+      <c r="F41" s="5"/>
+      <c r="G41" s="4"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D42" t="s">
+        <v>173</v>
+      </c>
+      <c r="G42" s="4"/>
+      <c r="H42" s="5"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D43" t="s">
+        <v>306</v>
+      </c>
+      <c r="G43" s="5"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="H44" s="5"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D45" t="s">
+        <v>203</v>
+      </c>
+      <c r="G45" s="5"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D46" t="s">
+        <v>308</v>
+      </c>
+      <c r="E46" s="4"/>
+      <c r="F46" s="5"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>4</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D47" t="s">
+        <v>304</v>
+      </c>
+      <c r="E47" s="4"/>
+      <c r="F47" s="5"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>4</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D48" t="s">
+        <v>305</v>
+      </c>
+      <c r="F48" s="4"/>
+      <c r="G48" s="5"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>4</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D49" t="s">
+        <v>246</v>
+      </c>
+      <c r="E49" s="5"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>4</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D50" t="s">
+        <v>257</v>
+      </c>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="4"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>4</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D51" t="s">
+        <v>251</v>
+      </c>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
+      <c r="H51" s="5"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>4</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D52" t="s">
+        <v>277</v>
+      </c>
+      <c r="E52" s="3"/>
+      <c r="G52" s="5"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>4</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D53" t="s">
+        <v>278</v>
+      </c>
+      <c r="E53" s="3"/>
+      <c r="F53" s="5"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>4</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D54" t="s">
+        <v>279</v>
+      </c>
+      <c r="F54" s="5"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>4</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D55" t="s">
+        <v>280</v>
+      </c>
+      <c r="E55" s="3"/>
+      <c r="F55" s="5"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>4</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D56" t="s">
+        <v>281</v>
+      </c>
+      <c r="E56" s="3"/>
+      <c r="F56" s="5"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>4</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D57" t="s">
+        <v>283</v>
+      </c>
+      <c r="E57" s="3"/>
+      <c r="F57" s="5"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>4</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D58" t="s">
+        <v>282</v>
+      </c>
+      <c r="E58" s="3"/>
+      <c r="F58" s="5"/>
+      <c r="G58" s="5"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>4</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D59" t="s">
+        <v>284</v>
+      </c>
+      <c r="G59" s="5"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>4</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D60" t="s">
+        <v>285</v>
+      </c>
+      <c r="F60" s="5"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>4</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D61" t="s">
+        <v>286</v>
+      </c>
+      <c r="E61" s="3"/>
+      <c r="F61" s="5"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>4</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D62" t="s">
+        <v>287</v>
+      </c>
+      <c r="E62" s="3"/>
+      <c r="G62" s="5"/>
+      <c r="H62" s="5"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>4</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D63" t="s">
+        <v>288</v>
+      </c>
+      <c r="E63" s="3"/>
+      <c r="G63" s="5"/>
+      <c r="H63" s="5"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>4</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="D64" t="s">
+        <v>289</v>
+      </c>
+      <c r="E64" s="3"/>
+      <c r="G64" s="7"/>
+      <c r="H64" s="5"/>
+    </row>
+    <row r="65" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E65" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60257923-960B-4E69-9BD4-B245B4366D96}">
   <dimension ref="A1:G150"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5146,57 +6432,59 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39BF42EB-875E-48DE-914B-2B24B20EF70D}">
-  <dimension ref="A1:E87"/>
+  <dimension ref="A1:H87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B68" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B48" sqref="B48"/>
+      <selection pane="bottomRight" activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="56.08984375" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="14.1796875" customWidth="1"/>
+    <col min="6" max="6" width="5.1796875" customWidth="1"/>
+    <col min="7" max="7" width="32.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B1" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C2" t="s">
         <v>189</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>190</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>191</v>
       </c>
-      <c r="E2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C3" t="s">
         <v>253</v>
-      </c>
-      <c r="C3" t="s">
-        <v>254</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
@@ -5205,63 +6493,92 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="E5" s="5"/>
+      <c r="G5" t="s">
+        <v>262</v>
+      </c>
+      <c r="H5" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>207</v>
-      </c>
-      <c r="E5" s="5"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>208</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G6" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G7" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="H7" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D8" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="G8" t="s">
+        <v>261</v>
+      </c>
+      <c r="H8" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G9" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G10" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>167</v>
       </c>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D12" s="5"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>168</v>
       </c>
@@ -5270,31 +6587,31 @@
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B17" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C17" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E17" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -5303,7 +6620,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="5"/>
@@ -5313,63 +6630,63 @@
         <v>172</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
@@ -5377,20 +6694,20 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E29" s="5"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
@@ -5398,42 +6715,42 @@
         <v>174</v>
       </c>
       <c r="B32" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="4"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
@@ -5444,22 +6761,22 @@
         <v>169</v>
       </c>
       <c r="B36" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="4"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
@@ -5467,77 +6784,77 @@
         <v>170</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="5"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B39" t="s">
+        <v>194</v>
+      </c>
+      <c r="C39" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="C39" s="4" t="s">
-        <v>196</v>
-      </c>
       <c r="D39" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E39" s="5"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B42" s="4"/>
       <c r="C42" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="5"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B47" s="4"/>
       <c r="C47" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E47" s="5"/>
     </row>
@@ -5548,57 +6865,57 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D50" s="5"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C51" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B52" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C52" s="5"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
@@ -5606,7 +6923,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
@@ -5624,16 +6941,16 @@
       </c>
       <c r="B58" s="4"/>
       <c r="C58" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D58" s="5"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D59" s="4"/>
     </row>
@@ -5652,7 +6969,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
@@ -5660,21 +6977,21 @@
         <v>176</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B65" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C65" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
@@ -5684,185 +7001,185 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C67" s="5"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B68" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C69" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D69" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
       <c r="D70" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B71" s="4"/>
       <c r="C71" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E71" s="4"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B72" s="4"/>
       <c r="C72" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D72" s="4"/>
       <c r="E72" s="5"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>178</v>
+        <v>268</v>
       </c>
       <c r="B75" s="3"/>
       <c r="D75" s="5"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B76" s="3"/>
       <c r="C76" s="5"/>
       <c r="D76" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B77" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C77" s="5"/>
       <c r="E77" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B78" s="3"/>
       <c r="C78" s="5"/>
       <c r="D78" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E78" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B79" s="3"/>
       <c r="C79" s="5"/>
       <c r="D79" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B80" s="3"/>
       <c r="C80" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B81" s="3"/>
       <c r="C81" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D81" s="5"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B82" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C82" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D82" s="5"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B83" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C83" s="5"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B84" s="3"/>
       <c r="C84" s="5"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B85" s="3"/>
       <c r="D85" s="5"/>
@@ -5870,14 +7187,14 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B86" s="3"/>
       <c r="D86" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E86" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>